<commit_message>
date format modification for Demogs and elastic
</commit_message>
<xml_diff>
--- a/yes-genie-testautomation-GenieDataCreation/src/main/resources/NBA.xlsx
+++ b/yes-genie-testautomation-GenieDataCreation/src/main/resources/NBA.xlsx
@@ -603,54 +603,46 @@
   </sheetPr>
   <dimension ref="A1:AN42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z10" activeCellId="0" sqref="Z10:Z13 Z31:Z34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="93.4132653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.6581632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="40.5"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="29.1581632653061"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="26.1887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="92.3367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="68.8469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="39.9591836734694"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="25.7857142857143"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +766,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -898,7 +890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1022,7 +1014,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -1146,7 +1138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1270,7 +1262,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
@@ -1394,7 +1386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
         <v>36</v>
       </c>
@@ -1518,7 +1510,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>39</v>
       </c>
@@ -1642,7 +1634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
         <v>42</v>
       </c>
@@ -1766,7 +1758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
         <v>45</v>
       </c>
@@ -1890,7 +1882,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
         <v>52</v>
       </c>
@@ -2014,7 +2006,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
         <v>54</v>
       </c>
@@ -2138,7 +2130,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
         <v>56</v>
       </c>
@@ -2262,7 +2254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
         <v>58</v>
       </c>
@@ -2386,7 +2378,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
         <v>65</v>
       </c>
@@ -2510,7 +2502,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
         <v>67</v>
       </c>
@@ -2634,7 +2626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
         <v>69</v>
       </c>
@@ -2758,7 +2750,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
         <v>71</v>
       </c>
@@ -2882,7 +2874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
         <v>76</v>
       </c>
@@ -3006,7 +2998,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
         <v>78</v>
       </c>
@@ -3130,7 +3122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
         <v>80</v>
       </c>
@@ -3254,7 +3246,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
@@ -3378,7 +3370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>83</v>
       </c>
@@ -3502,7 +3494,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>84</v>
       </c>
@@ -3626,7 +3618,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>85</v>
       </c>
@@ -3750,7 +3742,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
@@ -3874,7 +3866,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
         <v>87</v>
       </c>
@@ -3998,7 +3990,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
         <v>88</v>
       </c>
@@ -4122,7 +4114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
         <v>89</v>
       </c>
@@ -4246,7 +4238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
         <v>90</v>
       </c>
@@ -4370,7 +4362,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
         <v>91</v>
       </c>
@@ -4494,7 +4486,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
         <v>92</v>
       </c>
@@ -4618,7 +4610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
         <v>93</v>
       </c>
@@ -4742,7 +4734,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
         <v>94</v>
       </c>
@@ -4866,7 +4858,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
         <v>95</v>
       </c>
@@ -4990,7 +4982,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
         <v>96</v>
       </c>
@@ -5114,7 +5106,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
         <v>97</v>
       </c>
@@ -5238,7 +5230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
         <v>98</v>
       </c>
@@ -5362,7 +5354,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
         <v>99</v>
       </c>
@@ -5486,7 +5478,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
         <v>100</v>
       </c>
@@ -5610,7 +5602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
         <v>101</v>
       </c>
@@ -5734,7 +5726,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
         <v>102</v>
       </c>

</xml_diff>

<commit_message>
removing gradle from gitignore
</commit_message>
<xml_diff>
--- a/yes-genie-testautomation-GenieDataCreation/src/main/resources/NBA.xlsx
+++ b/yes-genie-testautomation-GenieDataCreation/src/main/resources/NBA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="151">
   <si>
     <t xml:space="preserve">row_key</t>
   </si>
@@ -298,169 +298,178 @@
     <t xml:space="preserve">Your FD is maturing, kindly reniew your FD(1)</t>
   </si>
   <si>
+    <t xml:space="preserve">FD02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alerts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your FD is maturing, kindly reniew your FD(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your FD is maturing, kindly reniew your FD(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-01-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your FD is maturing, kindly reniew your FD(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kindly Update email id and mobile no(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kindly Update email id and mobile no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kindly Update email id and mobile no(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kindly Update email id and mobile no(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kindly Update email id and mobile no(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"branch_code":"2","LOB":"Branch Banking","fd_amount":"54856.73","BU":"YES BANK"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FD03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-01-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MySpace/Reminders issue inquiry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-01-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-01-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issue Cheque Book (P 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update PAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAN01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-03-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-01-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issue Cheque Book (P 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dimiss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your FD is maturing, kindly reniew your FD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_142</t>
+  </si>
+  <si>
     <t xml:space="preserve">Renew FD</t>
   </si>
   <si>
-    <t xml:space="preserve">FD02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alerts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">996264849_137</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your FD is maturing, kindly reniew your FD(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">996264849_138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your FD is maturing, kindly reniew your FD(3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-01-26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">996264849_139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your FD is maturing, kindly reniew your FD(4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">996264849_140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kindly Update email id and mobile no(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAIL01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kindly Update email id and mobile no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">996264849_141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kindly Update email id and mobile no(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">996264849_142</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kindly Update email id and mobile no(3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">996264849_143</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kindly Update email id and mobile no(4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"branch_code":"2","LOB":"Branch Banking","fd_amount":"54856.73","BU":"YES BANK"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Issue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISSUE01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-01-21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MySpace/Reminders issue inquiry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-01-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-01-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Issue Cheque Book (P 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-03-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-01-28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Issue Cheque Book (P 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dimiss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_134</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_136</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your FD is maturing, kindly reniew your FD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_137</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_142</t>
+    <t xml:space="preserve">FD04</t>
   </si>
   <si>
     <t xml:space="preserve">998003452_143</t>
@@ -684,51 +693,51 @@
   </sheetPr>
   <dimension ref="A1:AN43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AK30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:AN43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2:S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="86.2602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="64.1224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="85.3163265306123"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.4438775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="37.7959183673469"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -909,8 +918,8 @@
         <v>47</v>
       </c>
       <c r="S2" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>48</v>
@@ -1033,8 +1042,8 @@
         <v>47</v>
       </c>
       <c r="S3" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>48</v>
@@ -1529,8 +1538,8 @@
         <v>47</v>
       </c>
       <c r="S7" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>48</v>
@@ -1653,8 +1662,8 @@
         <v>47</v>
       </c>
       <c r="S8" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>48</v>
@@ -2025,8 +2034,8 @@
         <v>47</v>
       </c>
       <c r="S11" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>79</v>
@@ -2149,8 +2158,8 @@
         <v>47</v>
       </c>
       <c r="S12" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>79</v>
@@ -2521,14 +2530,14 @@
         <v>47</v>
       </c>
       <c r="S15" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U15" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="V15" s="1" t="n">
         <f aca="false">0</f>
@@ -2544,7 +2553,7 @@
         <v>50</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA15" s="1" t="s">
         <v>52</v>
@@ -2591,7 +2600,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>996264849</v>
@@ -2612,7 +2621,7 @@
         <v>2</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I16" s="1" t="n">
         <v>996264849</v>
@@ -2645,30 +2654,30 @@
         <v>47</v>
       </c>
       <c r="S16" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U16" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="V16" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y16" s="1" t="s">
         <v>50</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA16" s="1" t="s">
         <v>52</v>
@@ -2715,7 +2724,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>996264849</v>
@@ -2736,7 +2745,7 @@
         <v>2</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I17" s="1" t="n">
         <v>996264849</v>
@@ -2773,26 +2782,26 @@
         <v>0</v>
       </c>
       <c r="T17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U17" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="V17" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y17" s="1" t="s">
         <v>50</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA17" s="1" t="s">
         <v>52</v>
@@ -2831,7 +2840,7 @@
         <v>58</v>
       </c>
       <c r="AM17" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AN17" s="1" t="s">
         <v>57</v>
@@ -2839,7 +2848,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>996264849</v>
@@ -2860,7 +2869,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I18" s="1" t="n">
         <v>996264849</v>
@@ -2897,26 +2906,26 @@
         <v>0</v>
       </c>
       <c r="T18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U18" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="V18" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA18" s="1" t="s">
         <v>52</v>
@@ -2963,7 +2972,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>996264849</v>
@@ -2984,7 +2993,7 @@
         <v>3</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I19" s="1" t="n">
         <v>996264849</v>
@@ -3017,24 +3026,24 @@
         <v>47</v>
       </c>
       <c r="S19" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="U19" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="U19" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="V19" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Y19" s="1" t="s">
         <v>50</v>
@@ -3087,7 +3096,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>996264849</v>
@@ -3108,7 +3117,7 @@
         <v>3</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I20" s="1" t="n">
         <v>996264849</v>
@@ -3145,20 +3154,20 @@
         <v>0</v>
       </c>
       <c r="T20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="U20" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="U20" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="V20" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Y20" s="1" t="s">
         <v>50</v>
@@ -3211,7 +3220,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>996264849</v>
@@ -3232,7 +3241,7 @@
         <v>3</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I21" s="1" t="n">
         <v>996264849</v>
@@ -3269,20 +3278,20 @@
         <v>0</v>
       </c>
       <c r="T21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="U21" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="U21" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="V21" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Y21" s="1" t="s">
         <v>50</v>
@@ -3335,7 +3344,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>996264849</v>
@@ -3356,7 +3365,7 @@
         <v>2</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I22" s="1" t="n">
         <v>996264849</v>
@@ -3389,24 +3398,24 @@
         <v>47</v>
       </c>
       <c r="S22" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="U22" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="U22" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="V22" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y22" s="1" t="s">
         <v>50</v>
@@ -3459,7 +3468,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>998003452</v>
@@ -3474,7 +3483,7 @@
         <v>41</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G23" s="1" t="n">
         <v>1</v>
@@ -3513,8 +3522,8 @@
         <v>47</v>
       </c>
       <c r="S23" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T23" s="1" t="s">
         <v>48</v>
@@ -3583,7 +3592,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>998003452</v>
@@ -3598,7 +3607,7 @@
         <v>41</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G24" s="1" t="n">
         <v>2</v>
@@ -3637,8 +3646,8 @@
         <v>47</v>
       </c>
       <c r="S24" s="8" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T24" s="1" t="s">
         <v>48</v>
@@ -3707,7 +3716,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>998003452</v>
@@ -3722,7 +3731,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G25" s="1" t="n">
         <v>3</v>
@@ -3831,7 +3840,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>998003452</v>
@@ -3846,7 +3855,7 @@
         <v>41</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G26" s="1" t="n">
         <v>4</v>
@@ -3955,7 +3964,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>998003452</v>
@@ -3970,7 +3979,7 @@
         <v>41</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G27" s="1" t="n">
         <v>5</v>
@@ -4079,7 +4088,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>998003452</v>
@@ -4094,7 +4103,7 @@
         <v>41</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G28" s="1" t="n">
         <v>4</v>
@@ -4137,10 +4146,10 @@
         <v>1</v>
       </c>
       <c r="T28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="U28" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="U28" s="9" t="s">
-        <v>121</v>
       </c>
       <c r="V28" s="1" t="n">
         <f aca="false">0</f>
@@ -4162,7 +4171,7 @@
         <v>52</v>
       </c>
       <c r="AB28" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AC28" s="1" t="n">
         <v>13</v>
@@ -4203,7 +4212,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>998003452</v>
@@ -4218,13 +4227,13 @@
         <v>41</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G29" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I29" s="1" t="n">
         <v>998003452</v>
@@ -4261,20 +4270,20 @@
         <v>1</v>
       </c>
       <c r="T29" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="U29" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="U29" s="9" t="s">
-        <v>121</v>
       </c>
       <c r="V29" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="X29" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Y29" s="1" t="s">
         <v>50</v>
@@ -4286,7 +4295,7 @@
         <v>52</v>
       </c>
       <c r="AB29" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AC29" s="1" t="n">
         <v>14</v>
@@ -4319,7 +4328,7 @@
         <v>58</v>
       </c>
       <c r="AM29" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AN29" s="1" t="s">
         <v>57</v>
@@ -4327,7 +4336,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>998003452</v>
@@ -4342,13 +4351,13 @@
         <v>41</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G30" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I30" s="1" t="n">
         <v>998003452</v>
@@ -4385,20 +4394,20 @@
         <v>0</v>
       </c>
       <c r="T30" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="U30" s="9" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="V30" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="X30" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Y30" s="1" t="s">
         <v>50</v>
@@ -4410,7 +4419,7 @@
         <v>52</v>
       </c>
       <c r="AB30" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AC30" s="1" t="n">
         <v>15</v>
@@ -4422,7 +4431,7 @@
         <v>46</v>
       </c>
       <c r="AF30" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AG30" s="1" t="s">
         <v>56</v>
@@ -4443,7 +4452,7 @@
         <v>58</v>
       </c>
       <c r="AM30" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AN30" s="1" t="s">
         <v>57</v>
@@ -4451,7 +4460,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>998003452</v>
@@ -4466,13 +4475,13 @@
         <v>41</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I31" s="1" t="n">
         <v>998003452</v>
@@ -4509,20 +4518,20 @@
         <v>0</v>
       </c>
       <c r="T31" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="U31" s="9" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="V31" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W31" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="X31" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Y31" s="1" t="s">
         <v>50</v>
@@ -4546,7 +4555,7 @@
         <v>46</v>
       </c>
       <c r="AF31" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AG31" s="1" t="s">
         <v>56</v>
@@ -4567,7 +4576,7 @@
         <v>58</v>
       </c>
       <c r="AM31" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AN31" s="1" t="s">
         <v>57</v>
@@ -4575,7 +4584,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>998003452</v>
@@ -4590,7 +4599,7 @@
         <v>41</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G32" s="1" t="n">
         <v>3</v>
@@ -4688,7 +4697,7 @@
         <v>57</v>
       </c>
       <c r="AL32" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AM32" s="5" t="s">
         <v>57</v>
@@ -4699,7 +4708,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>998003452</v>
@@ -4714,7 +4723,7 @@
         <v>41</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G33" s="1" t="n">
         <v>3</v>
@@ -4812,7 +4821,7 @@
         <v>57</v>
       </c>
       <c r="AL33" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AM33" s="5" t="s">
         <v>57</v>
@@ -4823,7 +4832,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>998003452</v>
@@ -4838,7 +4847,7 @@
         <v>41</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G34" s="1" t="n">
         <v>3</v>
@@ -4947,7 +4956,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>998003452</v>
@@ -4962,7 +4971,7 @@
         <v>41</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G35" s="1" t="n">
         <v>3</v>
@@ -5071,7 +5080,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>998003452</v>
@@ -5086,13 +5095,13 @@
         <v>41</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G36" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>998003452</v>
@@ -5129,26 +5138,26 @@
         <v>1</v>
       </c>
       <c r="T36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U36" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="V36" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W36" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="X36" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="Y36" s="1" t="s">
         <v>50</v>
       </c>
       <c r="Z36" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA36" s="1" t="s">
         <v>52</v>
@@ -5195,7 +5204,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>998003452</v>
@@ -5210,13 +5219,13 @@
         <v>41</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I37" s="1" t="n">
         <v>998003452</v>
@@ -5253,26 +5262,26 @@
         <v>1</v>
       </c>
       <c r="T37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U37" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="U37" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="V37" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W37" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X37" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y37" s="1" t="s">
         <v>50</v>
       </c>
       <c r="Z37" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA37" s="1" t="s">
         <v>52</v>
@@ -5319,7 +5328,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>998003452</v>
@@ -5334,13 +5343,13 @@
         <v>41</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G38" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I38" s="1" t="n">
         <v>998003452</v>
@@ -5377,26 +5386,26 @@
         <v>0</v>
       </c>
       <c r="T38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U38" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="U38" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="V38" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X38" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y38" s="1" t="s">
         <v>50</v>
       </c>
       <c r="Z38" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA38" s="1" t="s">
         <v>52</v>
@@ -5443,7 +5452,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>998003452</v>
@@ -5458,13 +5467,13 @@
         <v>41</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G39" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I39" s="1" t="n">
         <v>998003452</v>
@@ -5501,26 +5510,26 @@
         <v>0</v>
       </c>
       <c r="T39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U39" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="U39" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="V39" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y39" s="1" t="s">
         <v>50</v>
       </c>
       <c r="Z39" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA39" s="1" t="s">
         <v>52</v>
@@ -5567,7 +5576,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>998003452</v>
@@ -5582,13 +5591,13 @@
         <v>41</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G40" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I40" s="1" t="n">
         <v>998003452</v>
@@ -5625,20 +5634,20 @@
         <v>1</v>
       </c>
       <c r="T40" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="V40" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W40" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X40" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Y40" s="1" t="s">
         <v>50</v>
@@ -5691,7 +5700,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>998003452</v>
@@ -5706,13 +5715,13 @@
         <v>41</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G41" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I41" s="1" t="n">
         <v>998003452</v>
@@ -5749,20 +5758,20 @@
         <v>0</v>
       </c>
       <c r="T41" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U41" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="V41" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W41" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="X41" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Y41" s="1" t="s">
         <v>50</v>
@@ -5815,7 +5824,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>998003452</v>
@@ -5830,13 +5839,13 @@
         <v>41</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G42" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I42" s="1" t="n">
         <v>998003452</v>
@@ -5873,20 +5882,20 @@
         <v>0</v>
       </c>
       <c r="T42" s="1" t="s">
-        <v>104</v>
+        <v>148</v>
       </c>
       <c r="U42" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="V42" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W42" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X42" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Y42" s="1" t="s">
         <v>50</v>
@@ -5939,7 +5948,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>998003452</v>
@@ -5954,13 +5963,13 @@
         <v>41</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G43" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I43" s="1" t="n">
         <v>998003452</v>
@@ -5997,20 +6006,20 @@
         <v>1</v>
       </c>
       <c r="T43" s="1" t="s">
-        <v>104</v>
+        <v>148</v>
       </c>
       <c r="U43" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="V43" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="W43" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X43" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y43" s="1" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
adding portfolio details api
</commit_message>
<xml_diff>
--- a/yes-genie-testautomation-GenieDataCreation/src/main/resources/NBA.xlsx
+++ b/yes-genie-testautomation-GenieDataCreation/src/main/resources/NBA.xlsx
@@ -277,7 +277,7 @@
     <t xml:space="preserve">Book FD</t>
   </si>
   <si>
-    <t xml:space="preserve">FD01</t>
+    <t xml:space="preserve">FD001</t>
   </si>
   <si>
     <t xml:space="preserve">X-Sell</t>
@@ -316,7 +316,7 @@
     <t xml:space="preserve">Renew FD</t>
   </si>
   <si>
-    <t xml:space="preserve">FD02</t>
+    <t xml:space="preserve">FD002T</t>
   </si>
   <si>
     <t xml:space="preserve">Alerts</t>
@@ -352,7 +352,7 @@
     <t xml:space="preserve">Update Email</t>
   </si>
   <si>
-    <t xml:space="preserve">EMAIL01</t>
+    <t xml:space="preserve">Email001</t>
   </si>
   <si>
     <t xml:space="preserve">Kindly Update email id and mobile no</t>
@@ -475,9 +475,6 @@
     <t xml:space="preserve">998003452_140</t>
   </si>
   <si>
-    <t xml:space="preserve">Email01</t>
-  </si>
-  <si>
     <t xml:space="preserve">998003452_141</t>
   </si>
   <si>
@@ -530,6 +527,9 @@
   </si>
   <si>
     <t xml:space="preserve">update PAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAN001</t>
   </si>
   <si>
     <t xml:space="preserve">Kindly update your Permanent Account Number (PAN) as per regulation by Govt of India 1</t>
@@ -710,54 +710,55 @@
   </sheetPr>
   <dimension ref="A1:AR56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U56" activeCellId="0" sqref="U56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="79.6428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="58.9897959183674"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="63.7142857142857"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="43" min="41" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="45" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="78.6989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="58.3163265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="62.9081632653061"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="43" min="41" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="45" style="1" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6048,7 +6049,7 @@
         <v>109</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="V40" s="2" t="n">
         <v>0</v>
@@ -6122,7 +6123,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B41" s="2" t="n">
         <v>998003452</v>
@@ -6182,7 +6183,7 @@
         <v>109</v>
       </c>
       <c r="U41" s="2" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="V41" s="2" t="n">
         <v>0</v>
@@ -6256,7 +6257,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B42" s="2" t="n">
         <v>998003452</v>
@@ -6316,7 +6317,7 @@
         <v>109</v>
       </c>
       <c r="U42" s="2" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="V42" s="2" t="n">
         <v>0</v>
@@ -6390,7 +6391,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B43" s="2" t="n">
         <v>998003452</v>
@@ -6450,7 +6451,7 @@
         <v>109</v>
       </c>
       <c r="U43" s="2" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="V43" s="2" t="n">
         <v>0</v>
@@ -6524,7 +6525,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>1341527</v>
@@ -6539,13 +6540,13 @@
         <v>45</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G44" s="2" t="n">
         <v>4</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I44" s="2" t="n">
         <v>1341527</v>
@@ -6584,7 +6585,7 @@
         <v>50</v>
       </c>
       <c r="U44" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="V44" s="2" t="n">
         <v>0</v>
@@ -6658,7 +6659,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B45" s="2" t="n">
         <v>1341527</v>
@@ -6673,13 +6674,13 @@
         <v>45</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G45" s="2" t="n">
         <v>5</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I45" s="2" t="n">
         <v>1341527</v>
@@ -6718,7 +6719,7 @@
         <v>50</v>
       </c>
       <c r="U45" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="V45" s="2" t="n">
         <v>0</v>
@@ -6792,7 +6793,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B46" s="2" t="n">
         <v>1341527</v>
@@ -6804,16 +6805,16 @@
         <v>5</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G46" s="2" t="n">
         <v>3</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I46" s="2" t="n">
         <v>1341527</v>
@@ -6852,7 +6853,7 @@
         <v>50</v>
       </c>
       <c r="U46" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="V46" s="2" t="n">
         <v>0</v>
@@ -6926,7 +6927,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B47" s="2" t="n">
         <v>1341527</v>
@@ -6938,16 +6939,16 @@
         <v>5</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G47" s="2" t="n">
         <v>2</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I47" s="2" t="n">
         <v>1341527</v>
@@ -6986,7 +6987,7 @@
         <v>50</v>
       </c>
       <c r="U47" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="V47" s="2" t="n">
         <v>0</v>
@@ -7060,7 +7061,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B48" s="2" t="n">
         <v>1341527</v>
@@ -7072,16 +7073,16 @@
         <v>5</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G48" s="2" t="n">
         <v>1</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I48" s="2" t="n">
         <v>1341527</v>
@@ -7120,7 +7121,7 @@
         <v>50</v>
       </c>
       <c r="U48" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="V48" s="2" t="n">
         <v>0</v>
@@ -7194,7 +7195,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B49" s="2" t="n">
         <v>1341527</v>
@@ -7206,16 +7207,16 @@
         <v>1</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G49" s="2" t="n">
         <v>1</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I49" s="2" t="n">
         <v>1341527</v>
@@ -7236,7 +7237,7 @@
         <v>1341527</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P49" s="2" t="s">
         <v>50</v>
@@ -7341,13 +7342,13 @@
         <v>173</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G50" s="2" t="n">
         <v>2</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I50" s="2" t="n">
         <v>1341527</v>
@@ -7368,7 +7369,7 @@
         <v>1341527</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P50" s="2" t="s">
         <v>50</v>
@@ -7473,13 +7474,13 @@
         <v>176</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G51" s="2" t="n">
         <v>3</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I51" s="2" t="n">
         <v>1341527</v>
@@ -7500,7 +7501,7 @@
         <v>1341527</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P51" s="2" t="s">
         <v>50</v>
@@ -7605,13 +7606,13 @@
         <v>179</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G52" s="2" t="n">
         <v>1</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I52" s="2" t="n">
         <v>1341527</v>
@@ -7632,7 +7633,7 @@
         <v>1341527</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P52" s="2" t="s">
         <v>50</v>
@@ -7737,13 +7738,13 @@
         <v>182</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G53" s="2" t="n">
         <v>2</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I53" s="2" t="n">
         <v>1341527</v>
@@ -7764,7 +7765,7 @@
         <v>1341527</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P53" s="2" t="s">
         <v>50</v>
@@ -7869,13 +7870,13 @@
         <v>185</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G54" s="2" t="n">
         <v>2</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I54" s="2" t="n">
         <v>1341527</v>
@@ -7896,7 +7897,7 @@
         <v>1341527</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P54" s="2" t="s">
         <v>50</v>
@@ -8001,13 +8002,13 @@
         <v>188</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G55" s="2" t="n">
         <v>2</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I55" s="2" t="n">
         <v>1341527</v>
@@ -8028,7 +8029,7 @@
         <v>1341527</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P55" s="2" t="s">
         <v>50</v>
@@ -8133,13 +8134,13 @@
         <v>191</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G56" s="2" t="n">
         <v>2</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I56" s="2" t="n">
         <v>1341527</v>
@@ -8160,7 +8161,7 @@
         <v>1341527</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P56" s="2" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
NBA DATA Changes for recomadation end date
</commit_message>
<xml_diff>
--- a/yes-genie-testautomation-GenieDataCreation/src/main/resources/NBA.xlsx
+++ b/yes-genie-testautomation-GenieDataCreation/src/main/resources/NBA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="200">
   <si>
     <t xml:space="preserve">row_key</t>
   </si>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">CASE</t>
   </si>
   <si>
-    <t xml:space="preserve">2019-03-31</t>
+    <t xml:space="preserve">2021-03-31</t>
   </si>
   <si>
     <t xml:space="preserve">account</t>
@@ -452,9 +452,6 @@
   </si>
   <si>
     <t xml:space="preserve">Issue Cheque Book (P 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-03-24</t>
   </si>
   <si>
     <t xml:space="preserve">2019-01-28</t>
@@ -638,6 +635,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -725,56 +723,54 @@
   </sheetPr>
   <dimension ref="A1:AR56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE56" activeCellId="0" sqref="AE56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.6683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.6632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="73.6785714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.98469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.9030612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.2959183673469"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1530612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.4285714285714"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.3316326530612"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.515306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.2704081632653"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.5459183673469"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.0459183673469"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.2091836734694"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.2959183673469"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.40816326530612"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="73.9591836734694"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.3571428571429"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.3775510204082"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="23.9387755102041"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.98469387755102"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.4336734693878"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="23.2448979591837"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.6275510204082"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.7959183673469"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="13.6530612244898"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="14.0765306122449"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="22.8316326530612"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="11.1581632653061"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="13.1020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="45" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="72.8979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="73.1632653061225"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="45" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1539,7 +1535,7 @@
         <v>50</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="AF6" s="0" t="s">
         <v>60</v>
@@ -4621,7 +4617,7 @@
         <v>50</v>
       </c>
       <c r="AE29" s="1" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="AF29" s="0" t="s">
         <v>60</v>
@@ -4755,7 +4751,7 @@
         <v>50</v>
       </c>
       <c r="AE30" s="1" t="s">
-        <v>144</v>
+        <v>59</v>
       </c>
       <c r="AF30" s="0" t="s">
         <v>60</v>
@@ -4776,7 +4772,7 @@
         <v>62</v>
       </c>
       <c r="AL30" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM30" s="0" t="s">
         <v>61</v>
@@ -4799,7 +4795,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>998003452</v>
@@ -4820,7 +4816,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>998003452</v>
@@ -4865,10 +4861,10 @@
         <v>0</v>
       </c>
       <c r="W31" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="X31" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Y31" s="0" t="s">
         <v>120</v>
@@ -4889,7 +4885,7 @@
         <v>50</v>
       </c>
       <c r="AE31" s="1" t="s">
-        <v>144</v>
+        <v>59</v>
       </c>
       <c r="AF31" s="0" t="s">
         <v>60</v>
@@ -4910,7 +4906,7 @@
         <v>62</v>
       </c>
       <c r="AL31" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AM31" s="0" t="s">
         <v>61</v>
@@ -4933,7 +4929,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>998003452</v>
@@ -5041,7 +5037,7 @@
         <v>61</v>
       </c>
       <c r="AK32" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AL32" s="0" t="s">
         <v>61</v>
@@ -5067,7 +5063,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>998003452</v>
@@ -5175,7 +5171,7 @@
         <v>61</v>
       </c>
       <c r="AK33" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AL33" s="0" t="s">
         <v>61</v>
@@ -5201,7 +5197,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>998003452</v>
@@ -5335,7 +5331,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>998003452</v>
@@ -5469,7 +5465,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>998003452</v>
@@ -5490,7 +5486,7 @@
         <v>2</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>998003452</v>
@@ -5535,10 +5531,10 @@
         <v>0</v>
       </c>
       <c r="W36" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X36" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y36" s="0" t="s">
         <v>107</v>
@@ -5603,7 +5599,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>998003452</v>
@@ -5737,7 +5733,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>998003452</v>
@@ -5871,7 +5867,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>998003452</v>
@@ -6005,7 +6001,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>998003452</v>
@@ -6139,7 +6135,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>998003452</v>
@@ -6273,7 +6269,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>998003452</v>
@@ -6407,7 +6403,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>998003452</v>
@@ -6541,7 +6537,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1341527</v>
@@ -6556,13 +6552,13 @@
         <v>45</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G44" s="0" t="n">
         <v>4</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>1341527</v>
@@ -6601,7 +6597,7 @@
         <v>50</v>
       </c>
       <c r="U44" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V44" s="0" t="n">
         <v>0</v>
@@ -6675,7 +6671,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1341527</v>
@@ -6690,13 +6686,13 @@
         <v>45</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G45" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>1341527</v>
@@ -6735,7 +6731,7 @@
         <v>50</v>
       </c>
       <c r="U45" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V45" s="0" t="n">
         <v>0</v>
@@ -6809,7 +6805,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1341527</v>
@@ -6821,16 +6817,16 @@
         <v>5</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G46" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>1341527</v>
@@ -6869,7 +6865,7 @@
         <v>50</v>
       </c>
       <c r="U46" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V46" s="0" t="n">
         <v>0</v>
@@ -6943,7 +6939,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>1341527</v>
@@ -6955,16 +6951,16 @@
         <v>5</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G47" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>1341527</v>
@@ -7003,7 +6999,7 @@
         <v>50</v>
       </c>
       <c r="U47" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V47" s="0" t="n">
         <v>0</v>
@@ -7077,7 +7073,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1341527</v>
@@ -7089,16 +7085,16 @@
         <v>5</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>1341527</v>
@@ -7137,7 +7133,7 @@
         <v>50</v>
       </c>
       <c r="U48" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V48" s="0" t="n">
         <v>0</v>
@@ -7211,7 +7207,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1341527</v>
@@ -7223,16 +7219,16 @@
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G49" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I49" s="0" t="n">
         <v>1341527</v>
@@ -7253,7 +7249,7 @@
         <v>1341527</v>
       </c>
       <c r="O49" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P49" s="0" t="s">
         <v>50</v>
@@ -7271,16 +7267,16 @@
         <v>50</v>
       </c>
       <c r="U49" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="W49" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="W49" s="0" t="s">
+      <c r="X49" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y49" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="X49" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y49" s="0" t="s">
-        <v>179</v>
       </c>
       <c r="Z49" s="0" t="s">
         <v>56</v>
@@ -7342,7 +7338,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1341527</v>
@@ -7354,16 +7350,16 @@
         <v>1</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G50" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I50" s="0" t="n">
         <v>1341527</v>
@@ -7384,7 +7380,7 @@
         <v>1341527</v>
       </c>
       <c r="O50" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P50" s="0" t="s">
         <v>50</v>
@@ -7402,16 +7398,16 @@
         <v>50</v>
       </c>
       <c r="U50" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W50" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="X50" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Y50" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z50" s="0" t="s">
         <v>56</v>
@@ -7473,7 +7469,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>1341527</v>
@@ -7485,16 +7481,16 @@
         <v>1</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G51" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I51" s="0" t="n">
         <v>1341527</v>
@@ -7515,7 +7511,7 @@
         <v>1341527</v>
       </c>
       <c r="O51" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P51" s="0" t="s">
         <v>50</v>
@@ -7533,16 +7529,16 @@
         <v>50</v>
       </c>
       <c r="U51" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W51" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="X51" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Y51" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z51" s="0" t="s">
         <v>56</v>
@@ -7578,7 +7574,7 @@
         <v>61</v>
       </c>
       <c r="AK51" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AL51" s="0" t="s">
         <v>61</v>
@@ -7604,7 +7600,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>1341527</v>
@@ -7616,16 +7612,16 @@
         <v>1</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G52" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I52" s="0" t="n">
         <v>1341527</v>
@@ -7646,7 +7642,7 @@
         <v>1341527</v>
       </c>
       <c r="O52" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P52" s="0" t="s">
         <v>50</v>
@@ -7664,16 +7660,16 @@
         <v>50</v>
       </c>
       <c r="U52" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W52" s="0" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="X52" s="0" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Y52" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z52" s="0" t="s">
         <v>56</v>
@@ -7735,7 +7731,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>1341527</v>
@@ -7747,16 +7743,16 @@
         <v>1</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G53" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I53" s="0" t="n">
         <v>1341527</v>
@@ -7777,7 +7773,7 @@
         <v>1341527</v>
       </c>
       <c r="O53" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P53" s="0" t="s">
         <v>50</v>
@@ -7795,16 +7791,16 @@
         <v>50</v>
       </c>
       <c r="U53" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W53" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="X53" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Y53" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z53" s="0" t="s">
         <v>56</v>
@@ -7866,7 +7862,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1341527</v>
@@ -7878,16 +7874,16 @@
         <v>5</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G54" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I54" s="0" t="n">
         <v>1341527</v>
@@ -7908,7 +7904,7 @@
         <v>1341527</v>
       </c>
       <c r="O54" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P54" s="0" t="s">
         <v>50</v>
@@ -7926,16 +7922,16 @@
         <v>50</v>
       </c>
       <c r="U54" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W54" s="0" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="X54" s="0" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Y54" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z54" s="0" t="s">
         <v>56</v>
@@ -7997,7 +7993,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>1341527</v>
@@ -8009,16 +8005,16 @@
         <v>2</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G55" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I55" s="0" t="n">
         <v>1341527</v>
@@ -8039,7 +8035,7 @@
         <v>1341527</v>
       </c>
       <c r="O55" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P55" s="0" t="s">
         <v>50</v>
@@ -8057,16 +8053,16 @@
         <v>50</v>
       </c>
       <c r="U55" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W55" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="X55" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Y55" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z55" s="0" t="s">
         <v>56</v>
@@ -8128,7 +8124,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>1341527</v>
@@ -8140,16 +8136,16 @@
         <v>1</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G56" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I56" s="0" t="n">
         <v>1341527</v>
@@ -8170,7 +8166,7 @@
         <v>1341527</v>
       </c>
       <c r="O56" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P56" s="0" t="s">
         <v>50</v>
@@ -8188,16 +8184,16 @@
         <v>50</v>
       </c>
       <c r="U56" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W56" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="X56" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Y56" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z56" s="0" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
api changes for UAT
</commit_message>
<xml_diff>
--- a/yes-genie-testautomation-GenieDataCreation/src/main/resources/NBA.xlsx
+++ b/yes-genie-testautomation-GenieDataCreation/src/main/resources/NBA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="197">
   <si>
     <t xml:space="preserve">row_key</t>
   </si>
@@ -160,7 +160,7 @@
     <t xml:space="preserve">2018-12-14</t>
   </si>
   <si>
-    <t xml:space="preserve">{"branch_code":"1","lob":"Branch Banking","amount":"54856.73","due_date":"2019-03-31"}</t>
+    <t xml:space="preserve">{"branch_code":"1","lob":"Branch Banking","amount":"54856.73","due_date":"2019-11-31"}</t>
   </si>
   <si>
     <t xml:space="preserve">Cash not or less dispensed from Domestic Other bank ATM but account debited</t>
@@ -181,10 +181,10 @@
     <t xml:space="preserve">FALSE</t>
   </si>
   <si>
-    <t xml:space="preserve">Create SR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SA002T</t>
+    <t xml:space="preserve">Update FATCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FATCA</t>
   </si>
   <si>
     <t xml:space="preserve">Regulatory</t>
@@ -199,18 +199,21 @@
     <t xml:space="preserve">CASE</t>
   </si>
   <si>
+    <t xml:space="preserve">2019-03-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEN</t>
+  </si>
+  <si>
     <t xml:space="preserve">2021-03-31</t>
   </si>
   <si>
-    <t xml:space="preserve">account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEN</t>
-  </si>
-  <si>
     <t xml:space="preserve">996264849_124</t>
   </si>
   <si>
@@ -220,9 +223,6 @@
     <t xml:space="preserve">CA</t>
   </si>
   <si>
-    <t xml:space="preserve">CA002T</t>
-  </si>
-  <si>
     <t xml:space="preserve">996264849_125</t>
   </si>
   <si>
@@ -232,9 +232,6 @@
     <t xml:space="preserve">PL</t>
   </si>
   <si>
-    <t xml:space="preserve">PL002T</t>
-  </si>
-  <si>
     <t xml:space="preserve">996264849_126</t>
   </si>
   <si>
@@ -244,9 +241,6 @@
     <t xml:space="preserve">MF</t>
   </si>
   <si>
-    <t xml:space="preserve">MF002T</t>
-  </si>
-  <si>
     <t xml:space="preserve">996264849_127</t>
   </si>
   <si>
@@ -256,9 +250,6 @@
     <t xml:space="preserve">FD</t>
   </si>
   <si>
-    <t xml:space="preserve">SR01</t>
-  </si>
-  <si>
     <t xml:space="preserve">2019-01-25</t>
   </si>
   <si>
@@ -334,13 +325,10 @@
     <t xml:space="preserve">996264849_136</t>
   </si>
   <si>
-    <t xml:space="preserve">Your FD is maturing, kindly reniew your FD(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renew FD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FD002T</t>
+    <t xml:space="preserve">You have need of locker, kindly request a locker(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locker001</t>
   </si>
   <si>
     <t xml:space="preserve">Alerts</t>
@@ -349,150 +337,159 @@
     <t xml:space="preserve">996264849_137</t>
   </si>
   <si>
+    <t xml:space="preserve">You have need of locker, kindly request a locker(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have need of locker, kindly request a locker(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-01-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have need of locker, kindly request a locker(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kindly Update email id and mobile no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kindly Update email id and mobile no(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kindly Update email id and mobile no(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">996264849_143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kindly Update email id and mobile no(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"branch_code":"2","lob":"Branch Banking","amount":"54856.73","due_date":"2019-11-31"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplication for installation of POS(Point of Sale) Machine(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POS001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-01-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplication for installation of POS(Point of Sale) Machine(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-01-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-01-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplication for installation of POS(Point of Sale) Machine(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-01-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplication for installation of POS(Point of Sale) Machine(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISMISSED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your FD is maturing, kindly reniew your FD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSME001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998003452_137</t>
+  </si>
+  <si>
     <t xml:space="preserve">Your FD is maturing, kindly reniew your FD(2)</t>
   </si>
   <si>
-    <t xml:space="preserve">996264849_138</t>
+    <t xml:space="preserve">998003452_138</t>
   </si>
   <si>
     <t xml:space="preserve">Your FD is maturing, kindly reniew your FD(3)</t>
   </si>
   <si>
-    <t xml:space="preserve">2019-01-26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">996264849_139</t>
+    <t xml:space="preserve">998003452_139</t>
   </si>
   <si>
     <t xml:space="preserve">Your FD is maturing, kindly reniew your FD(4)</t>
   </si>
   <si>
-    <t xml:space="preserve">996264849_140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kindly Update email id and mobile no(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kindly Update email id and mobile no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">996264849_141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kindly Update email id and mobile no(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">996264849_142</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kindly Update email id and mobile no(3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">996264849_143</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kindly Update email id and mobile no(4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"branch_code":"2","lob":"Branch Banking","amount":"54856.73","due_date":"2019-03-31"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Issue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISSUE01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-01-21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MySpace/Reminders issue inquiry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-01-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-01-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Issue Cheque Book (P 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-01-28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Issue Cheque Book (P 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISMISSED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_134</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_136</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your FD is maturing, kindly reniew your FD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_137</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">998003452_139</t>
-  </si>
-  <si>
     <t xml:space="preserve">998003452_140</t>
   </si>
   <si>
@@ -508,10 +505,7 @@
     <t xml:space="preserve">1179699_10715447929060</t>
   </si>
   <si>
-    <t xml:space="preserve">{"branch_code":"3","lob":"Branch Banking","amount":"54856.73","due_date":"2019-03-31"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dear SURESHKUMAR TRIVEDI Your FD is about to expire ,Please Renew</t>
+    <t xml:space="preserve">{"branch_code":"3","lob":"Branch Banking","amount":"54856.73","due_date":"2019-11-31"}</t>
   </si>
   <si>
     <t xml:space="preserve">FD_Renew</t>
@@ -544,16 +538,13 @@
     <t xml:space="preserve">2018-12-18</t>
   </si>
   <si>
-    <t xml:space="preserve">Dear KUSUM LATA GUPTA ,Your PAN is not Updated ,Please Update ASAP</t>
+    <t xml:space="preserve">Kindly update your Permanent Account Number (PAN) as per regulation by Govt of India 1</t>
   </si>
   <si>
     <t xml:space="preserve">update PAN</t>
   </si>
   <si>
     <t xml:space="preserve">PAN001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kindly update your Permanent Account Number (PAN) as per regulation by Govt of India 1</t>
   </si>
   <si>
     <t xml:space="preserve">Regulatory </t>
@@ -723,54 +714,55 @@
   </sheetPr>
   <dimension ref="A1:AR56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE56" activeCellId="0" sqref="AE56"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="72.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="73.1632653061225"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="23.6224489795918"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="45" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="71.9489795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="64.2551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="72.3571428571429"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="12.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,8 +1020,8 @@
       <c r="AN2" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO2" s="0" t="s">
-        <v>61</v>
+      <c r="AO2" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP2" s="0" t="n">
         <v>0</v>
@@ -1043,7 +1035,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>996264849</v>
@@ -1064,7 +1056,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>996264849</v>
@@ -1094,7 +1086,7 @@
         <v>107</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>52</v>
@@ -1103,16 +1095,16 @@
         <v>53</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="V3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Y3" s="0" t="s">
         <v>55</v>
@@ -1162,8 +1154,8 @@
       <c r="AN3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO3" s="0" t="s">
-        <v>61</v>
+      <c r="AO3" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP3" s="0" t="n">
         <v>0</v>
@@ -1237,7 +1229,7 @@
         <v>53</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="V4" s="0" t="n">
         <v>0</v>
@@ -1296,8 +1288,8 @@
       <c r="AN4" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO4" s="0" t="s">
-        <v>61</v>
+      <c r="AO4" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP4" s="0" t="n">
         <v>0</v>
@@ -1311,7 +1303,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>996264849</v>
@@ -1332,7 +1324,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>996264849</v>
@@ -1362,7 +1354,7 @@
         <v>107</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>52</v>
@@ -1371,16 +1363,16 @@
         <v>53</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="V5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Y5" s="0" t="s">
         <v>55</v>
@@ -1430,8 +1422,8 @@
       <c r="AN5" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO5" s="0" t="s">
-        <v>61</v>
+      <c r="AO5" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP5" s="0" t="n">
         <v>0</v>
@@ -1445,7 +1437,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>996264849</v>
@@ -1466,7 +1458,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>996264849</v>
@@ -1496,7 +1488,7 @@
         <v>107</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>52</v>
@@ -1505,16 +1497,16 @@
         <v>53</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="V6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Y6" s="0" t="s">
         <v>55</v>
@@ -1523,7 +1515,7 @@
         <v>56</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AB6" s="0" t="n">
         <v>133</v>
@@ -1564,8 +1556,8 @@
       <c r="AN6" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO6" s="0" t="s">
-        <v>61</v>
+      <c r="AO6" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP6" s="0" t="n">
         <v>0</v>
@@ -1579,7 +1571,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>996264849</v>
@@ -1600,7 +1592,7 @@
         <v>4</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>996264849</v>
@@ -1630,25 +1622,25 @@
         <v>107</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T7" s="0" t="s">
         <v>53</v>
       </c>
       <c r="U7" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="V7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W7" s="0" t="s">
-        <v>81</v>
-      </c>
       <c r="X7" s="0" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Y7" s="0" t="s">
         <v>55</v>
@@ -1657,7 +1649,7 @@
         <v>56</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AB7" s="0" t="n">
         <v>208</v>
@@ -1698,8 +1690,8 @@
       <c r="AN7" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO7" s="0" t="s">
-        <v>61</v>
+      <c r="AO7" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP7" s="0" t="n">
         <v>0</v>
@@ -1713,7 +1705,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>996264849</v>
@@ -1734,7 +1726,7 @@
         <v>3</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>996264849</v>
@@ -1764,25 +1756,25 @@
         <v>107</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T8" s="0" t="s">
         <v>53</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="V8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Y8" s="0" t="s">
         <v>55</v>
@@ -1791,7 +1783,7 @@
         <v>56</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AB8" s="0" t="n">
         <v>391</v>
@@ -1832,8 +1824,8 @@
       <c r="AN8" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO8" s="0" t="s">
-        <v>61</v>
+      <c r="AO8" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP8" s="0" t="n">
         <v>0</v>
@@ -1847,7 +1839,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>996264849</v>
@@ -1868,7 +1860,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>996264849</v>
@@ -1898,7 +1890,7 @@
         <v>107</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>52</v>
@@ -1907,16 +1899,16 @@
         <v>53</v>
       </c>
       <c r="U9" s="0" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="V9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="X9" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="Y9" s="0" t="s">
         <v>55</v>
@@ -1925,7 +1917,7 @@
         <v>56</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AB9" s="0" t="n">
         <v>516</v>
@@ -1966,8 +1958,8 @@
       <c r="AN9" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO9" s="0" t="s">
-        <v>61</v>
+      <c r="AO9" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP9" s="0" t="n">
         <v>0</v>
@@ -1981,7 +1973,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>996264849</v>
@@ -2002,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>996264849</v>
@@ -2032,7 +2024,7 @@
         <v>107</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>52</v>
@@ -2041,16 +2033,16 @@
         <v>53</v>
       </c>
       <c r="U10" s="0" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="V10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="X10" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="Y10" s="0" t="s">
         <v>55</v>
@@ -2059,7 +2051,7 @@
         <v>56</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AB10" s="0" t="n">
         <v>168</v>
@@ -2100,8 +2092,8 @@
       <c r="AN10" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO10" s="0" t="s">
-        <v>61</v>
+      <c r="AO10" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP10" s="0" t="n">
         <v>0</v>
@@ -2115,7 +2107,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>996264849</v>
@@ -2136,7 +2128,7 @@
         <v>3</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>996264849</v>
@@ -2166,40 +2158,40 @@
         <v>107</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T11" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W11" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="X11" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y11" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="X11" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y11" s="0" t="s">
-        <v>94</v>
       </c>
       <c r="Z11" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AC11" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD11" s="0" t="s">
         <v>50</v>
@@ -2232,10 +2224,10 @@
         <v>61</v>
       </c>
       <c r="AN11" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO11" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="AO11" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP11" s="0" t="n">
         <v>0</v>
@@ -2249,7 +2241,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>996264849</v>
@@ -2270,7 +2262,7 @@
         <v>3</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>996264849</v>
@@ -2300,40 +2292,40 @@
         <v>107</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U12" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="X12" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="Y12" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Z12" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AC12" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD12" s="0" t="s">
         <v>50</v>
@@ -2366,10 +2358,10 @@
         <v>61</v>
       </c>
       <c r="AN12" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO12" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="AO12" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP12" s="0" t="n">
         <v>0</v>
@@ -2383,7 +2375,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>996264849</v>
@@ -2404,7 +2396,7 @@
         <v>3</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>996264849</v>
@@ -2434,40 +2426,40 @@
         <v>107</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U13" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="X13" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Y13" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Z13" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB13" s="0" t="n">
         <v>3</v>
       </c>
       <c r="AC13" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD13" s="0" t="s">
         <v>50</v>
@@ -2500,10 +2492,10 @@
         <v>61</v>
       </c>
       <c r="AN13" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO13" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="AO13" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP13" s="0" t="n">
         <v>0</v>
@@ -2517,7 +2509,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>996264849</v>
@@ -2538,7 +2530,7 @@
         <v>3</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>996264849</v>
@@ -2568,40 +2560,40 @@
         <v>107</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T14" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U14" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W14" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="X14" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Y14" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Z14" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB14" s="0" t="n">
         <v>4</v>
       </c>
       <c r="AC14" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD14" s="0" t="s">
         <v>50</v>
@@ -2634,10 +2626,10 @@
         <v>61</v>
       </c>
       <c r="AN14" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO14" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="AO14" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP14" s="0" t="n">
         <v>0</v>
@@ -2651,7 +2643,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>996264849</v>
@@ -2672,7 +2664,7 @@
         <v>2</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>996264849</v>
@@ -2702,40 +2694,40 @@
         <v>107</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T15" s="0" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="U15" s="0" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="V15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W15" s="0" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="X15" s="0" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="Y15" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="Z15" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB15" s="0" t="n">
         <v>5</v>
       </c>
       <c r="AC15" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD15" s="0" t="s">
         <v>50</v>
@@ -2768,10 +2760,10 @@
         <v>61</v>
       </c>
       <c r="AN15" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO15" s="0" t="s">
-        <v>61</v>
+        <v>103</v>
+      </c>
+      <c r="AO15" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP15" s="0" t="n">
         <v>0</v>
@@ -2785,7 +2777,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>996264849</v>
@@ -2806,7 +2798,7 @@
         <v>2</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>996264849</v>
@@ -2836,40 +2828,40 @@
         <v>107</v>
       </c>
       <c r="R16" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T16" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="U16" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="U16" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="V16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W16" s="0" t="s">
-        <v>109</v>
-      </c>
       <c r="X16" s="0" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="Y16" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="Z16" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB16" s="0" t="n">
         <v>6</v>
       </c>
       <c r="AC16" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD16" s="0" t="s">
         <v>50</v>
@@ -2902,10 +2894,10 @@
         <v>61</v>
       </c>
       <c r="AN16" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO16" s="0" t="s">
-        <v>61</v>
+        <v>103</v>
+      </c>
+      <c r="AO16" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP16" s="0" t="n">
         <v>0</v>
@@ -2919,7 +2911,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>996264849</v>
@@ -2940,7 +2932,7 @@
         <v>2</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>996264849</v>
@@ -2970,40 +2962,40 @@
         <v>107</v>
       </c>
       <c r="R17" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T17" s="0" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="U17" s="0" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="V17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="X17" s="0" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Y17" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="Z17" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB17" s="0" t="n">
         <v>7</v>
       </c>
       <c r="AC17" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD17" s="0" t="s">
         <v>50</v>
@@ -3030,16 +3022,16 @@
         <v>62</v>
       </c>
       <c r="AL17" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="AM17" s="0" t="s">
         <v>61</v>
       </c>
       <c r="AN17" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO17" s="0" t="s">
-        <v>61</v>
+        <v>103</v>
+      </c>
+      <c r="AO17" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP17" s="0" t="n">
         <v>0</v>
@@ -3053,7 +3045,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>996264849</v>
@@ -3074,7 +3066,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>996264849</v>
@@ -3104,40 +3096,40 @@
         <v>107</v>
       </c>
       <c r="R18" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T18" s="0" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="V18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W18" s="0" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="X18" s="0" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="Y18" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="Z18" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB18" s="0" t="n">
         <v>8</v>
       </c>
       <c r="AC18" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD18" s="0" t="s">
         <v>50</v>
@@ -3170,10 +3162,10 @@
         <v>61</v>
       </c>
       <c r="AN18" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO18" s="0" t="s">
-        <v>61</v>
+        <v>103</v>
+      </c>
+      <c r="AO18" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP18" s="0" t="n">
         <v>0</v>
@@ -3187,7 +3179,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>996264849</v>
@@ -3208,7 +3200,7 @@
         <v>3</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>996264849</v>
@@ -3238,40 +3230,40 @@
         <v>107</v>
       </c>
       <c r="R19" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T19" s="0" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="V19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W19" s="0" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="X19" s="0" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="Y19" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Z19" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB19" s="0" t="n">
         <v>9</v>
       </c>
       <c r="AC19" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD19" s="0" t="s">
         <v>50</v>
@@ -3304,10 +3296,10 @@
         <v>61</v>
       </c>
       <c r="AN19" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="AO19" s="0" t="s">
-        <v>61</v>
+        <v>116</v>
+      </c>
+      <c r="AO19" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP19" s="0" t="n">
         <v>0</v>
@@ -3321,7 +3313,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>996264849</v>
@@ -3342,7 +3334,7 @@
         <v>3</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>996264849</v>
@@ -3372,40 +3364,40 @@
         <v>107</v>
       </c>
       <c r="R20" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T20" s="0" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="U20" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="V20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="V20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W20" s="0" t="s">
-        <v>116</v>
-      </c>
       <c r="X20" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="Y20" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Z20" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB20" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AC20" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD20" s="0" t="s">
         <v>50</v>
@@ -3438,10 +3430,10 @@
         <v>61</v>
       </c>
       <c r="AN20" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="AO20" s="0" t="s">
-        <v>61</v>
+        <v>116</v>
+      </c>
+      <c r="AO20" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP20" s="0" t="n">
         <v>0</v>
@@ -3455,7 +3447,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>996264849</v>
@@ -3476,7 +3468,7 @@
         <v>3</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>996264849</v>
@@ -3506,40 +3498,40 @@
         <v>107</v>
       </c>
       <c r="R21" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T21" s="0" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="U21" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="V21" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W21" s="0" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="X21" s="0" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Y21" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Z21" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA21" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB21" s="0" t="n">
         <v>11</v>
       </c>
       <c r="AC21" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD21" s="0" t="s">
         <v>50</v>
@@ -3572,10 +3564,10 @@
         <v>61</v>
       </c>
       <c r="AN21" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="AO21" s="0" t="s">
-        <v>61</v>
+        <v>116</v>
+      </c>
+      <c r="AO21" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP21" s="0" t="n">
         <v>0</v>
@@ -3589,7 +3581,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>996264849</v>
@@ -3610,7 +3602,7 @@
         <v>2</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>996264849</v>
@@ -3640,40 +3632,40 @@
         <v>107</v>
       </c>
       <c r="R22" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T22" s="0" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="U22" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="V22" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W22" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="X22" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="Y22" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Z22" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB22" s="0" t="n">
         <v>12</v>
       </c>
       <c r="AC22" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD22" s="0" t="s">
         <v>50</v>
@@ -3706,10 +3698,10 @@
         <v>61</v>
       </c>
       <c r="AN22" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO22" s="0" t="s">
-        <v>61</v>
+        <v>115</v>
+      </c>
+      <c r="AO22" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP22" s="0" t="n">
         <v>0</v>
@@ -3723,7 +3715,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>998003452</v>
@@ -3738,7 +3730,7 @@
         <v>45</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>1</v>
@@ -3774,16 +3766,16 @@
         <v>107</v>
       </c>
       <c r="R23" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T23" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="U23" s="0" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="V23" s="0" t="n">
         <v>0</v>
@@ -3801,7 +3793,7 @@
         <v>56</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AB23" s="0" t="n">
         <v>9</v>
@@ -3857,7 +3849,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>998003452</v>
@@ -3872,13 +3864,13 @@
         <v>45</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>998003452</v>
@@ -3908,25 +3900,25 @@
         <v>107</v>
       </c>
       <c r="R24" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T24" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="U24" s="0" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="V24" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W24" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="X24" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Y24" s="0" t="s">
         <v>55</v>
@@ -3935,7 +3927,7 @@
         <v>56</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AB24" s="0" t="n">
         <v>15</v>
@@ -3976,8 +3968,8 @@
       <c r="AN24" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO24" s="0" t="s">
-        <v>61</v>
+      <c r="AO24" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP24" s="0" t="n">
         <v>0</v>
@@ -3991,7 +3983,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>998003452</v>
@@ -4006,7 +3998,7 @@
         <v>45</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>3</v>
@@ -4042,16 +4034,16 @@
         <v>107</v>
       </c>
       <c r="R25" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S25" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T25" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="U25" s="0" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="V25" s="0" t="n">
         <v>0</v>
@@ -4069,7 +4061,7 @@
         <v>56</v>
       </c>
       <c r="AA25" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AB25" s="0" t="n">
         <v>927</v>
@@ -4110,8 +4102,8 @@
       <c r="AN25" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO25" s="0" t="s">
-        <v>61</v>
+      <c r="AO25" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP25" s="0" t="n">
         <v>0</v>
@@ -4125,7 +4117,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>998003452</v>
@@ -4140,13 +4132,13 @@
         <v>45</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>4</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>998003452</v>
@@ -4176,25 +4168,25 @@
         <v>107</v>
       </c>
       <c r="R26" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S26" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T26" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="U26" s="0" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="V26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W26" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="X26" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Y26" s="0" t="s">
         <v>55</v>
@@ -4203,7 +4195,7 @@
         <v>56</v>
       </c>
       <c r="AA26" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AB26" s="0" t="n">
         <v>139</v>
@@ -4244,8 +4236,8 @@
       <c r="AN26" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO26" s="0" t="s">
-        <v>61</v>
+      <c r="AO26" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP26" s="0" t="n">
         <v>0</v>
@@ -4259,7 +4251,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>998003452</v>
@@ -4274,13 +4266,13 @@
         <v>45</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>998003452</v>
@@ -4310,25 +4302,25 @@
         <v>107</v>
       </c>
       <c r="R27" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T27" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="U27" s="0" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="V27" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W27" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="X27" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Y27" s="0" t="s">
         <v>55</v>
@@ -4337,7 +4329,7 @@
         <v>56</v>
       </c>
       <c r="AA27" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AB27" s="0" t="n">
         <v>133</v>
@@ -4378,8 +4370,8 @@
       <c r="AN27" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO27" s="0" t="s">
-        <v>61</v>
+      <c r="AO27" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP27" s="0" t="n">
         <v>0</v>
@@ -4393,7 +4385,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>998003452</v>
@@ -4408,13 +4400,13 @@
         <v>45</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>4</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>998003452</v>
@@ -4444,40 +4436,40 @@
         <v>107</v>
       </c>
       <c r="R28" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T28" s="0" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="U28" s="0" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="V28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W28" s="0" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="X28" s="0" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="Y28" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Z28" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA28" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="AB28" s="0" t="n">
         <v>13</v>
       </c>
       <c r="AC28" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD28" s="0" t="s">
         <v>50</v>
@@ -4510,7 +4502,7 @@
         <v>61</v>
       </c>
       <c r="AN28" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="AO28" s="0" t="s">
         <v>61</v>
@@ -4527,7 +4519,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>998003452</v>
@@ -4542,13 +4534,13 @@
         <v>45</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>998003452</v>
@@ -4578,40 +4570,40 @@
         <v>107</v>
       </c>
       <c r="R29" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T29" s="0" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="U29" s="0" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="V29" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W29" s="0" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="X29" s="0" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="Y29" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Z29" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA29" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="AB29" s="0" t="n">
         <v>14</v>
       </c>
       <c r="AC29" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD29" s="0" t="s">
         <v>50</v>
@@ -4638,16 +4630,16 @@
         <v>62</v>
       </c>
       <c r="AL29" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="AM29" s="0" t="s">
         <v>61</v>
       </c>
       <c r="AN29" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO29" s="0" t="s">
-        <v>61</v>
+        <v>115</v>
+      </c>
+      <c r="AO29" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP29" s="0" t="n">
         <v>0</v>
@@ -4661,7 +4653,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>998003452</v>
@@ -4676,13 +4668,13 @@
         <v>45</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>998003452</v>
@@ -4712,40 +4704,40 @@
         <v>107</v>
       </c>
       <c r="R30" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S30" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T30" s="0" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="U30" s="0" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="V30" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W30" s="0" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="X30" s="0" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="Y30" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Z30" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA30" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="AB30" s="0" t="n">
         <v>15</v>
       </c>
       <c r="AC30" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD30" s="0" t="s">
         <v>50</v>
@@ -4772,16 +4764,16 @@
         <v>62</v>
       </c>
       <c r="AL30" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="AM30" s="0" t="s">
         <v>61</v>
       </c>
       <c r="AN30" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO30" s="0" t="s">
-        <v>61</v>
+        <v>115</v>
+      </c>
+      <c r="AO30" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP30" s="0" t="n">
         <v>0</v>
@@ -4795,7 +4787,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>998003452</v>
@@ -4810,13 +4802,13 @@
         <v>45</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>998003452</v>
@@ -4846,28 +4838,28 @@
         <v>107</v>
       </c>
       <c r="R31" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S31" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T31" s="0" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="U31" s="0" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="V31" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W31" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="X31" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="Y31" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Z31" s="0" t="s">
         <v>56</v>
@@ -4879,7 +4871,7 @@
         <v>16</v>
       </c>
       <c r="AC31" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD31" s="0" t="s">
         <v>50</v>
@@ -4906,16 +4898,16 @@
         <v>62</v>
       </c>
       <c r="AL31" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="AM31" s="0" t="s">
         <v>61</v>
       </c>
       <c r="AN31" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO31" s="0" t="s">
-        <v>61</v>
+        <v>115</v>
+      </c>
+      <c r="AO31" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP31" s="0" t="n">
         <v>0</v>
@@ -4929,7 +4921,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>998003452</v>
@@ -4944,13 +4936,13 @@
         <v>45</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>998003452</v>
@@ -4980,40 +4972,40 @@
         <v>107</v>
       </c>
       <c r="R32" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T32" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U32" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V32" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W32" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="X32" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Y32" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Z32" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA32" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB32" s="0" t="n">
         <v>17</v>
       </c>
       <c r="AC32" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD32" s="0" t="s">
         <v>50</v>
@@ -5037,7 +5029,7 @@
         <v>61</v>
       </c>
       <c r="AK32" s="0" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AL32" s="0" t="s">
         <v>61</v>
@@ -5046,10 +5038,10 @@
         <v>61</v>
       </c>
       <c r="AN32" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO32" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="AO32" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP32" s="0" t="n">
         <v>0</v>
@@ -5063,7 +5055,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>998003452</v>
@@ -5078,13 +5070,13 @@
         <v>45</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>998003452</v>
@@ -5114,28 +5106,28 @@
         <v>107</v>
       </c>
       <c r="R33" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T33" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U33" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W33" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="X33" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Y33" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Z33" s="0" t="s">
         <v>56</v>
@@ -5147,7 +5139,7 @@
         <v>18</v>
       </c>
       <c r="AC33" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD33" s="0" t="s">
         <v>50</v>
@@ -5171,7 +5163,7 @@
         <v>61</v>
       </c>
       <c r="AK33" s="0" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AL33" s="0" t="s">
         <v>61</v>
@@ -5180,10 +5172,10 @@
         <v>61</v>
       </c>
       <c r="AN33" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO33" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="AO33" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP33" s="0" t="n">
         <v>0</v>
@@ -5197,7 +5189,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>998003452</v>
@@ -5212,13 +5204,13 @@
         <v>45</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>998003452</v>
@@ -5248,28 +5240,28 @@
         <v>107</v>
       </c>
       <c r="R34" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S34" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T34" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U34" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V34" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W34" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="X34" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Y34" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Z34" s="0" t="s">
         <v>56</v>
@@ -5281,7 +5273,7 @@
         <v>19</v>
       </c>
       <c r="AC34" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD34" s="0" t="s">
         <v>50</v>
@@ -5314,7 +5306,7 @@
         <v>61</v>
       </c>
       <c r="AN34" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="AO34" s="0" t="s">
         <v>61</v>
@@ -5331,7 +5323,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>998003452</v>
@@ -5346,13 +5338,13 @@
         <v>45</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G35" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>998003452</v>
@@ -5382,28 +5374,28 @@
         <v>107</v>
       </c>
       <c r="R35" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S35" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T35" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U35" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V35" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W35" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="X35" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Y35" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Z35" s="0" t="s">
         <v>56</v>
@@ -5415,7 +5407,7 @@
         <v>20</v>
       </c>
       <c r="AC35" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD35" s="0" t="s">
         <v>50</v>
@@ -5448,10 +5440,10 @@
         <v>61</v>
       </c>
       <c r="AN35" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO35" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="AO35" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP35" s="0" t="n">
         <v>0</v>
@@ -5465,7 +5457,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>998003452</v>
@@ -5480,13 +5472,13 @@
         <v>45</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>998003452</v>
@@ -5516,28 +5508,28 @@
         <v>107</v>
       </c>
       <c r="R36" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T36" s="0" t="s">
-        <v>105</v>
+        <v>149</v>
       </c>
       <c r="U36" s="0" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="V36" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W36" s="0" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="X36" s="0" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="Y36" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="Z36" s="0" t="s">
         <v>56</v>
@@ -5549,7 +5541,7 @@
         <v>21</v>
       </c>
       <c r="AC36" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD36" s="0" t="s">
         <v>50</v>
@@ -5582,10 +5574,10 @@
         <v>61</v>
       </c>
       <c r="AN36" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO36" s="0" t="s">
-        <v>61</v>
+        <v>103</v>
+      </c>
+      <c r="AO36" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP36" s="0" t="n">
         <v>0</v>
@@ -5599,7 +5591,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>998003452</v>
@@ -5614,13 +5606,13 @@
         <v>45</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>998003452</v>
@@ -5650,28 +5642,28 @@
         <v>107</v>
       </c>
       <c r="R37" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S37" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T37" s="0" t="s">
-        <v>105</v>
+        <v>149</v>
       </c>
       <c r="U37" s="0" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="V37" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W37" s="0" t="s">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="X37" s="0" t="s">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="Y37" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="Z37" s="0" t="s">
         <v>56</v>
@@ -5683,7 +5675,7 @@
         <v>22</v>
       </c>
       <c r="AC37" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD37" s="0" t="s">
         <v>50</v>
@@ -5716,10 +5708,10 @@
         <v>61</v>
       </c>
       <c r="AN37" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO37" s="0" t="s">
-        <v>61</v>
+        <v>103</v>
+      </c>
+      <c r="AO37" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP37" s="0" t="n">
         <v>0</v>
@@ -5733,7 +5725,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>998003452</v>
@@ -5748,13 +5740,13 @@
         <v>45</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G38" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>998003452</v>
@@ -5784,28 +5776,28 @@
         <v>107</v>
       </c>
       <c r="R38" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S38" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T38" s="0" t="s">
-        <v>105</v>
+        <v>149</v>
       </c>
       <c r="U38" s="0" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="V38" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W38" s="0" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="X38" s="0" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="Y38" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="Z38" s="0" t="s">
         <v>56</v>
@@ -5817,7 +5809,7 @@
         <v>23</v>
       </c>
       <c r="AC38" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD38" s="0" t="s">
         <v>50</v>
@@ -5850,10 +5842,10 @@
         <v>61</v>
       </c>
       <c r="AN38" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO38" s="0" t="s">
-        <v>61</v>
+        <v>103</v>
+      </c>
+      <c r="AO38" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP38" s="0" t="n">
         <v>0</v>
@@ -5867,7 +5859,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>998003452</v>
@@ -5882,13 +5874,13 @@
         <v>45</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G39" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>114</v>
+        <v>155</v>
       </c>
       <c r="I39" s="0" t="n">
         <v>998003452</v>
@@ -5918,28 +5910,28 @@
         <v>107</v>
       </c>
       <c r="R39" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S39" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T39" s="0" t="s">
-        <v>105</v>
+        <v>149</v>
       </c>
       <c r="U39" s="0" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="V39" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W39" s="0" t="s">
-        <v>114</v>
+        <v>155</v>
       </c>
       <c r="X39" s="0" t="s">
-        <v>114</v>
+        <v>155</v>
       </c>
       <c r="Y39" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="Z39" s="0" t="s">
         <v>56</v>
@@ -5951,7 +5943,7 @@
         <v>24</v>
       </c>
       <c r="AC39" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD39" s="0" t="s">
         <v>50</v>
@@ -5984,10 +5976,10 @@
         <v>61</v>
       </c>
       <c r="AN39" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO39" s="0" t="s">
-        <v>61</v>
+        <v>103</v>
+      </c>
+      <c r="AO39" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP39" s="0" t="n">
         <v>0</v>
@@ -6001,7 +5993,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>998003452</v>
@@ -6016,13 +6008,13 @@
         <v>45</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G40" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>998003452</v>
@@ -6052,28 +6044,28 @@
         <v>107</v>
       </c>
       <c r="R40" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S40" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T40" s="0" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="U40" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="V40" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W40" s="0" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="X40" s="0" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="Y40" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Z40" s="0" t="s">
         <v>56</v>
@@ -6085,7 +6077,7 @@
         <v>25</v>
       </c>
       <c r="AC40" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD40" s="0" t="s">
         <v>50</v>
@@ -6118,10 +6110,10 @@
         <v>61</v>
       </c>
       <c r="AN40" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="AO40" s="0" t="s">
-        <v>61</v>
+        <v>116</v>
+      </c>
+      <c r="AO40" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP40" s="0" t="n">
         <v>0</v>
@@ -6135,7 +6127,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>998003452</v>
@@ -6150,13 +6142,13 @@
         <v>45</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G41" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>998003452</v>
@@ -6186,28 +6178,28 @@
         <v>107</v>
       </c>
       <c r="R41" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S41" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T41" s="0" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="U41" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="V41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W41" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="V41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W41" s="0" t="s">
-        <v>116</v>
-      </c>
       <c r="X41" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="Y41" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Z41" s="0" t="s">
         <v>56</v>
@@ -6219,7 +6211,7 @@
         <v>26</v>
       </c>
       <c r="AC41" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD41" s="0" t="s">
         <v>50</v>
@@ -6252,10 +6244,10 @@
         <v>61</v>
       </c>
       <c r="AN41" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="AO41" s="0" t="s">
-        <v>61</v>
+        <v>116</v>
+      </c>
+      <c r="AO41" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP41" s="0" t="n">
         <v>0</v>
@@ -6269,7 +6261,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>998003452</v>
@@ -6284,13 +6276,13 @@
         <v>45</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G42" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>998003452</v>
@@ -6320,28 +6312,28 @@
         <v>107</v>
       </c>
       <c r="R42" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S42" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T42" s="0" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="U42" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="V42" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W42" s="0" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="X42" s="0" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Y42" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Z42" s="0" t="s">
         <v>56</v>
@@ -6353,7 +6345,7 @@
         <v>27</v>
       </c>
       <c r="AC42" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD42" s="0" t="s">
         <v>50</v>
@@ -6386,10 +6378,10 @@
         <v>61</v>
       </c>
       <c r="AN42" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO42" s="0" t="s">
-        <v>61</v>
+        <v>115</v>
+      </c>
+      <c r="AO42" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP42" s="0" t="n">
         <v>0</v>
@@ -6403,7 +6395,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>998003452</v>
@@ -6418,13 +6410,13 @@
         <v>45</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G43" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I43" s="0" t="n">
         <v>998003452</v>
@@ -6454,28 +6446,28 @@
         <v>107</v>
       </c>
       <c r="R43" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S43" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T43" s="0" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="U43" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="V43" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W43" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="X43" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="Y43" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Z43" s="0" t="s">
         <v>56</v>
@@ -6487,7 +6479,7 @@
         <v>28</v>
       </c>
       <c r="AC43" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD43" s="0" t="s">
         <v>50</v>
@@ -6520,10 +6512,10 @@
         <v>61</v>
       </c>
       <c r="AN43" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO43" s="0" t="s">
-        <v>61</v>
+        <v>115</v>
+      </c>
+      <c r="AO43" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP43" s="0" t="n">
         <v>0</v>
@@ -6537,7 +6529,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1341527</v>
@@ -6552,13 +6544,13 @@
         <v>45</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G44" s="0" t="n">
         <v>4</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>1341527</v>
@@ -6588,40 +6580,40 @@
         <v>107</v>
       </c>
       <c r="R44" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S44" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T44" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U44" s="0" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="V44" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W44" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="X44" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y44" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="X44" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y44" s="0" t="s">
-        <v>94</v>
       </c>
       <c r="Z44" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA44" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AC44" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD44" s="0" t="s">
         <v>50</v>
@@ -6654,10 +6646,10 @@
         <v>61</v>
       </c>
       <c r="AN44" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO44" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="AO44" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP44" s="0" t="n">
         <v>0</v>
@@ -6671,7 +6663,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1341527</v>
@@ -6686,13 +6678,13 @@
         <v>45</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G45" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>163</v>
+        <v>95</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>1341527</v>
@@ -6722,40 +6714,40 @@
         <v>107</v>
       </c>
       <c r="R45" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T45" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U45" s="0" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="V45" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W45" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="X45" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="Y45" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Z45" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA45" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB45" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AC45" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD45" s="0" t="s">
         <v>50</v>
@@ -6788,10 +6780,10 @@
         <v>61</v>
       </c>
       <c r="AN45" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO45" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="AO45" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP45" s="0" t="n">
         <v>0</v>
@@ -6805,7 +6797,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1341527</v>
@@ -6817,16 +6809,16 @@
         <v>5</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G46" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>163</v>
+        <v>97</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>1341527</v>
@@ -6856,40 +6848,40 @@
         <v>107</v>
       </c>
       <c r="R46" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T46" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U46" s="0" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="V46" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W46" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="X46" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Y46" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Z46" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA46" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB46" s="0" t="n">
         <v>3</v>
       </c>
       <c r="AC46" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD46" s="0" t="s">
         <v>50</v>
@@ -6922,10 +6914,10 @@
         <v>61</v>
       </c>
       <c r="AN46" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO46" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="AO46" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP46" s="0" t="n">
         <v>0</v>
@@ -6939,7 +6931,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>1341527</v>
@@ -6951,16 +6943,16 @@
         <v>5</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G47" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>1341527</v>
@@ -6990,40 +6982,40 @@
         <v>107</v>
       </c>
       <c r="R47" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S47" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T47" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U47" s="0" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="V47" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W47" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="X47" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Y47" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Z47" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA47" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB47" s="0" t="n">
         <v>4</v>
       </c>
       <c r="AC47" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD47" s="0" t="s">
         <v>50</v>
@@ -7056,10 +7048,10 @@
         <v>61</v>
       </c>
       <c r="AN47" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO47" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="AO47" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP47" s="0" t="n">
         <v>0</v>
@@ -7073,7 +7065,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1341527</v>
@@ -7085,16 +7077,16 @@
         <v>5</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>1341527</v>
@@ -7124,40 +7116,40 @@
         <v>107</v>
       </c>
       <c r="R48" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S48" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T48" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U48" s="0" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="V48" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W48" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="X48" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Y48" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Z48" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA48" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB48" s="0" t="n">
         <v>5</v>
       </c>
       <c r="AC48" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AD48" s="0" t="s">
         <v>50</v>
@@ -7190,10 +7182,10 @@
         <v>61</v>
       </c>
       <c r="AN48" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO48" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
+      </c>
+      <c r="AO48" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP48" s="0" t="n">
         <v>0</v>
@@ -7207,7 +7199,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1341527</v>
@@ -7219,16 +7211,16 @@
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G49" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I49" s="0" t="n">
         <v>1341527</v>
@@ -7249,7 +7241,7 @@
         <v>1341527</v>
       </c>
       <c r="O49" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P49" s="0" t="s">
         <v>50</v>
@@ -7258,31 +7250,31 @@
         <v>108</v>
       </c>
       <c r="R49" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S49" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T49" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U49" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W49" s="0" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="X49" s="0" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="Y49" s="0" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z49" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA49" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB49" s="0" t="n">
         <v>9</v>
@@ -7323,8 +7315,8 @@
       <c r="AN49" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO49" s="0" t="s">
-        <v>61</v>
+      <c r="AO49" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP49" s="0" t="n">
         <v>0</v>
@@ -7338,7 +7330,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1341527</v>
@@ -7350,16 +7342,16 @@
         <v>1</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G50" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="I50" s="0" t="n">
         <v>1341527</v>
@@ -7380,7 +7372,7 @@
         <v>1341527</v>
       </c>
       <c r="O50" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P50" s="0" t="s">
         <v>50</v>
@@ -7389,31 +7381,31 @@
         <v>109</v>
       </c>
       <c r="R50" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S50" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T50" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U50" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W50" s="0" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="X50" s="0" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Y50" s="0" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z50" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA50" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB50" s="0" t="n">
         <v>15</v>
@@ -7454,8 +7446,8 @@
       <c r="AN50" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO50" s="0" t="s">
-        <v>61</v>
+      <c r="AO50" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP50" s="0" t="n">
         <v>0</v>
@@ -7469,7 +7461,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>1341527</v>
@@ -7481,16 +7473,16 @@
         <v>1</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G51" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="I51" s="0" t="n">
         <v>1341527</v>
@@ -7511,7 +7503,7 @@
         <v>1341527</v>
       </c>
       <c r="O51" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P51" s="0" t="s">
         <v>50</v>
@@ -7520,31 +7512,31 @@
         <v>110</v>
       </c>
       <c r="R51" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T51" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U51" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W51" s="0" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="X51" s="0" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="Y51" s="0" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z51" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA51" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB51" s="0" t="n">
         <v>927</v>
@@ -7574,7 +7566,7 @@
         <v>61</v>
       </c>
       <c r="AK51" s="0" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AL51" s="0" t="s">
         <v>61</v>
@@ -7585,8 +7577,8 @@
       <c r="AN51" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO51" s="0" t="s">
-        <v>61</v>
+      <c r="AO51" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP51" s="0" t="n">
         <v>0</v>
@@ -7600,7 +7592,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>1341527</v>
@@ -7612,16 +7604,16 @@
         <v>1</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G52" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="I52" s="0" t="n">
         <v>1341527</v>
@@ -7642,7 +7634,7 @@
         <v>1341527</v>
       </c>
       <c r="O52" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P52" s="0" t="s">
         <v>50</v>
@@ -7651,31 +7643,31 @@
         <v>111</v>
       </c>
       <c r="R52" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S52" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T52" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U52" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W52" s="0" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="X52" s="0" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="Y52" s="0" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z52" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA52" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB52" s="0" t="n">
         <v>139</v>
@@ -7716,8 +7708,8 @@
       <c r="AN52" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO52" s="0" t="s">
-        <v>61</v>
+      <c r="AO52" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP52" s="0" t="n">
         <v>0</v>
@@ -7731,7 +7723,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>1341527</v>
@@ -7743,16 +7735,16 @@
         <v>1</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G53" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="I53" s="0" t="n">
         <v>1341527</v>
@@ -7773,7 +7765,7 @@
         <v>1341527</v>
       </c>
       <c r="O53" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P53" s="0" t="s">
         <v>50</v>
@@ -7782,31 +7774,31 @@
         <v>112</v>
       </c>
       <c r="R53" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S53" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T53" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U53" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W53" s="0" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="X53" s="0" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="Y53" s="0" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z53" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA53" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB53" s="0" t="n">
         <v>133</v>
@@ -7847,8 +7839,8 @@
       <c r="AN53" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO53" s="0" t="s">
-        <v>61</v>
+      <c r="AO53" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP53" s="0" t="n">
         <v>0</v>
@@ -7862,7 +7854,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1341527</v>
@@ -7874,16 +7866,16 @@
         <v>5</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G54" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="I54" s="0" t="n">
         <v>1341527</v>
@@ -7904,7 +7896,7 @@
         <v>1341527</v>
       </c>
       <c r="O54" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P54" s="0" t="s">
         <v>50</v>
@@ -7913,31 +7905,31 @@
         <v>113</v>
       </c>
       <c r="R54" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S54" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T54" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U54" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W54" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="X54" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="Y54" s="0" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z54" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA54" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB54" s="0" t="n">
         <v>208</v>
@@ -7978,8 +7970,8 @@
       <c r="AN54" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO54" s="0" t="s">
-        <v>61</v>
+      <c r="AO54" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP54" s="0" t="n">
         <v>0</v>
@@ -7993,7 +7985,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>1341527</v>
@@ -8005,16 +7997,16 @@
         <v>2</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G55" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="I55" s="0" t="n">
         <v>1341527</v>
@@ -8035,7 +8027,7 @@
         <v>1341527</v>
       </c>
       <c r="O55" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P55" s="0" t="s">
         <v>50</v>
@@ -8044,31 +8036,31 @@
         <v>114</v>
       </c>
       <c r="R55" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T55" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U55" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W55" s="0" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="X55" s="0" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Y55" s="0" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z55" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA55" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB55" s="0" t="n">
         <v>391</v>
@@ -8109,8 +8101,8 @@
       <c r="AN55" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO55" s="0" t="s">
-        <v>61</v>
+      <c r="AO55" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP55" s="0" t="n">
         <v>0</v>
@@ -8124,7 +8116,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>1341527</v>
@@ -8136,16 +8128,16 @@
         <v>1</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G56" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="I56" s="0" t="n">
         <v>1341527</v>
@@ -8166,7 +8158,7 @@
         <v>1341527</v>
       </c>
       <c r="O56" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P56" s="0" t="s">
         <v>50</v>
@@ -8175,31 +8167,31 @@
         <v>115</v>
       </c>
       <c r="R56" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="T56" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U56" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="W56" s="0" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="X56" s="0" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="Y56" s="0" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z56" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA56" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB56" s="0" t="n">
         <v>516</v>
@@ -8240,8 +8232,8 @@
       <c r="AN56" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="AO56" s="0" t="s">
-        <v>61</v>
+      <c r="AO56" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="AP56" s="0" t="n">
         <v>0</v>

</xml_diff>